<commit_message>
SNF Error Fixing p.1
</commit_message>
<xml_diff>
--- a/error_report/Error Report Inpatient.xlsx
+++ b/error_report/Error Report Inpatient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="758">
   <si>
     <t>05/05 to 05/11</t>
   </si>
@@ -2287,6 +2287,9 @@
   </si>
   <si>
     <t>Member Termed at Auth</t>
+  </si>
+  <si>
+    <t>Swing Bed No Total Amount</t>
   </si>
 </sst>
 </file>
@@ -2366,7 +2369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2384,9 +2387,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2725,8 +2725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H437"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="F260" sqref="F260"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,3353 +2770,3507 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>946686</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>917905</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>42837</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>947249</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>936475</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>42839</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>917905</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>917905</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="12">
         <v>42843</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>920553</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>936409</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>939409</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>939409</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>42850</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>948000</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>936475</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>42488</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>945268</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>936475</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>42773</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>910639</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>903408</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>42781</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>911023</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>915731</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>42793</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>935086</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>936439</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>920534</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>920534</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>903798</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>912043</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>947611</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>947611</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>913771</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>900155</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>937585</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <v>920184</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="12">
         <v>42808</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>902070</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>904635</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>903807</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>936497</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <v>42810</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>917687</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>936416</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <v>42809</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>921985</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>936469</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>910893</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>920176</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <v>42860</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>920184</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>920534</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>933409</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <v>906239</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="12">
         <v>42808</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>907047</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="10">
         <v>936497</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="11">
         <v>42813</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>933409</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="10">
         <v>906239</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="11">
         <v>42818</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>908708</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="10">
         <v>933332</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="11">
         <v>42822</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>901308</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="8">
         <v>900155</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="12">
         <v>42823</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>907044</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="8">
         <v>927026</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="12">
         <v>42823</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>903999</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="8">
         <v>945237</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="12">
         <v>42827</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <v>908708</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="10">
         <v>904201</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="11">
         <v>42829</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <v>911689</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="8">
         <v>923693</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="12">
         <v>42828</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="7" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>937101</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <v>920184</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="12">
         <v>42861</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <v>948831</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="8">
         <v>936400</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="12">
         <v>42832</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <v>928193</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="8">
         <v>906239</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="12">
         <v>42835</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <v>937109</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="8">
         <v>936439</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="12">
         <v>42836</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <v>906079</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="8">
         <v>920184</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="12">
         <v>42845</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <v>918203</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="8">
         <v>936421</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="12">
         <v>42836</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10">
         <v>911060</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="10">
         <v>906239</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G38" s="12">
+      <c r="G38" s="11">
         <v>42838</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <v>934629</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="8">
         <v>934629</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <v>911533</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="8">
         <v>936416</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="G40" s="13">
+      <c r="G40" s="12">
         <v>42839</v>
       </c>
-      <c r="H40" s="9" t="s">
+      <c r="H40" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8">
         <v>947084</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="8">
         <v>936461</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="12">
         <v>42841</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="H41" s="7" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <v>904970</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="8">
         <v>999999</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F42" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G42" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="8" t="s">
+      <c r="H42" s="7" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8">
         <v>948317</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="8">
         <v>906699</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="12">
         <v>42839</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="7" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="8">
         <v>947610</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="8">
         <v>936421</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="12">
         <v>42839</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="10">
         <v>923188</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D45" s="10">
         <v>936402</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="11">
         <v>42842</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="H45" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="8">
         <v>907238</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="8">
         <v>906699</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="G46" s="13">
+      <c r="G46" s="12">
         <v>42839</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="H46" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="8">
         <v>934844</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="8">
         <v>948436</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G47" s="13">
+      <c r="G47" s="12">
         <v>42635</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H47" s="7" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="10">
         <v>936477</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D48" s="10">
         <v>936477</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="H48" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="10">
         <v>902070</v>
       </c>
-      <c r="D49" s="11">
+      <c r="D49" s="10">
         <v>904635</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H49" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="8">
         <v>999999999</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="8">
         <v>920306</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="H50" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="10">
         <v>913830</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="10">
         <v>936416</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G51" s="12">
+      <c r="G51" s="11">
         <v>42848</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="H51" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="10">
         <v>911533</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="10">
         <v>936446</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="11" t="s">
+      <c r="G52" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H52" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="8">
         <v>925373</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="8">
         <v>936486</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="F53" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G53" s="13">
+      <c r="G53" s="12">
         <v>42856</v>
       </c>
-      <c r="H53" s="8" t="s">
+      <c r="H53" s="7" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="10">
         <v>922113</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="10">
         <v>929440</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G54" s="12">
+      <c r="G54" s="11">
         <v>42849</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="10">
         <v>912283</v>
       </c>
-      <c r="D55" s="11">
+      <c r="D55" s="10">
         <v>936446</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="10" t="s">
+      <c r="H55" s="9" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="8">
         <v>912793</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="8">
         <v>936416</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G56" s="13">
+      <c r="G56" s="12">
         <v>42853</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C57" s="8">
         <v>902363</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="8">
         <v>906699</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G57" s="13">
+      <c r="G57" s="12">
         <v>42854</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="H57" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C58" s="8">
         <v>911533</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="8">
         <v>936416</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="G58" s="13">
+      <c r="G58" s="12">
         <v>42853</v>
       </c>
-      <c r="H58" s="9" t="s">
+      <c r="H58" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C59" s="8">
         <v>922046</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="8">
         <v>920580</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G59" s="13">
+      <c r="G59" s="12">
         <v>42488</v>
       </c>
-      <c r="H59" s="9" t="s">
+      <c r="H59" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="8">
         <v>914385</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="8">
         <v>936416</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F60" s="9" t="s">
+      <c r="F60" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="G60" s="13">
+      <c r="G60" s="12">
         <v>42857</v>
       </c>
-      <c r="H60" s="8" t="s">
+      <c r="H60" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="8">
         <v>904235</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="8">
         <v>936439</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F61" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G61" s="13">
+      <c r="G61" s="12">
         <v>42853</v>
       </c>
-      <c r="H61" s="8" t="s">
+      <c r="H61" s="7" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="8">
         <v>935114</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="8">
         <v>920184</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="12">
         <v>42856</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="H62" s="8" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C63" s="8">
         <v>936932</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D63" s="8">
         <v>920157</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E63" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F63" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="12">
         <v>42857</v>
       </c>
-      <c r="H63" s="8" t="s">
+      <c r="H63" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C64" s="8">
         <v>943144</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D64" s="8">
         <v>920157</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="12">
         <v>42858</v>
       </c>
-      <c r="H64" s="8" t="s">
+      <c r="H64" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C65" s="8">
         <v>900736</v>
       </c>
-      <c r="D65" s="9">
+      <c r="D65" s="8">
         <v>939279</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F65" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="12">
         <v>42857</v>
       </c>
-      <c r="H65" s="9" t="s">
+      <c r="H65" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="8">
         <v>902070</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D66" s="8">
         <v>904635</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="12">
         <v>42858</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="H66" s="8" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="8">
         <v>922046</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="8">
         <v>920580</v>
       </c>
-      <c r="E67" s="9" t="s">
+      <c r="E67" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G67" s="13">
+      <c r="G67" s="12">
         <v>42861</v>
       </c>
-      <c r="H67" s="9" t="s">
+      <c r="H67" s="8" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C68" s="8">
         <v>936922</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D68" s="8">
         <v>920184</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="E68" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G68" s="13">
+      <c r="G68" s="12">
         <v>42860</v>
       </c>
-      <c r="H68" s="8" t="s">
+      <c r="H68" s="7" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C69" s="8">
         <v>944179</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="8">
         <v>936409</v>
       </c>
-      <c r="E69" s="9" t="s">
+      <c r="E69" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G69" s="13">
+      <c r="G69" s="12">
         <v>42863</v>
       </c>
-      <c r="H69" s="8" t="s">
+      <c r="H69" s="7" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C70" s="8">
         <v>903798</v>
       </c>
-      <c r="D70" s="9">
+      <c r="D70" s="8">
         <v>912043</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G70" s="13">
+      <c r="G70" s="12">
         <v>42866</v>
       </c>
-      <c r="H70" s="8" t="s">
+      <c r="H70" s="7" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C71" s="8">
         <v>935546</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="8">
         <v>936533</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F71" s="6" t="s">
+      <c r="E71" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F71" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G71" s="7">
+      <c r="G71" s="12">
         <v>42773</v>
       </c>
-      <c r="H71" s="6"/>
+      <c r="H71" s="7" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C72" s="6">
+      <c r="C72" s="8">
         <v>941835</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72" s="8">
         <v>913334</v>
       </c>
-      <c r="E72" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F72" s="6" t="s">
+      <c r="E72" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F72" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G72" s="7">
+      <c r="G72" s="12">
         <v>42785</v>
       </c>
-      <c r="H72" s="6"/>
+      <c r="H72" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C73" s="6">
+      <c r="C73" s="8">
         <v>900819</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="8">
         <v>936526</v>
       </c>
-      <c r="E73" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F73" s="6" t="s">
+      <c r="E73" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F73" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G73" s="7">
+      <c r="G73" s="12">
         <v>42787</v>
       </c>
-      <c r="H73" s="6"/>
+      <c r="H73" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C74" s="8">
         <v>927490</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="8">
         <v>913334</v>
       </c>
-      <c r="E74" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F74" s="6" t="s">
+      <c r="E74" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F74" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="G74" s="7">
+      <c r="G74" s="12">
         <v>42821</v>
       </c>
-      <c r="H74" s="6"/>
+      <c r="H74" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C75" s="6">
+      <c r="C75" s="10">
         <v>935696</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75" s="10">
         <v>902590</v>
       </c>
-      <c r="E75" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F75" s="6" t="s">
+      <c r="E75" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F75" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="G75" s="7">
+      <c r="G75" s="11">
         <v>42790</v>
       </c>
-      <c r="H75" s="6"/>
+      <c r="H75" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C76" s="6">
+      <c r="C76" s="10">
         <v>936993</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76" s="10">
         <v>939400</v>
       </c>
-      <c r="E76" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F76" s="6" t="s">
+      <c r="E76" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F76" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="G76" s="7">
+      <c r="G76" s="11">
         <v>42795</v>
       </c>
-      <c r="H76" s="6"/>
+      <c r="H76" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="6">
+      <c r="C77" s="10">
         <v>908403</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77" s="10">
         <v>942462</v>
       </c>
-      <c r="E77" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F77" s="6" t="s">
+      <c r="E77" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F77" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G77" s="11">
         <v>42795</v>
       </c>
-      <c r="H77" s="6"/>
+      <c r="H77" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C78" s="10">
         <v>936993</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78" s="10">
         <v>939400</v>
       </c>
-      <c r="E78" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F78" s="6" t="s">
+      <c r="E78" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F78" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="G78" s="7">
+      <c r="G78" s="11">
         <v>42797</v>
       </c>
-      <c r="H78" s="6"/>
+      <c r="H78" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C79" s="10">
         <v>928964</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79" s="10">
         <v>928713</v>
       </c>
-      <c r="E79" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F79" s="6" t="s">
+      <c r="E79" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F79" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G79" s="11">
         <v>42801</v>
       </c>
-      <c r="H79" s="6"/>
+      <c r="H79" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C80" s="6">
+      <c r="C80" s="10">
         <v>908403</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80" s="10">
         <v>942462</v>
       </c>
-      <c r="E80" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F80" s="6" t="s">
+      <c r="E80" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F80" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G80" s="7">
+      <c r="G80" s="11">
         <v>42796</v>
       </c>
-      <c r="H80" s="6"/>
+      <c r="H80" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C81" s="6">
+      <c r="C81" s="8">
         <v>922103</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81" s="8">
         <v>949769</v>
       </c>
-      <c r="E81" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F81" s="6" t="s">
+      <c r="E81" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F81" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="G81" s="7">
+      <c r="G81" s="12">
         <v>42804</v>
       </c>
-      <c r="H81" s="6"/>
+      <c r="H81" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C82" s="10">
         <v>905904</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="10">
         <v>920011</v>
       </c>
-      <c r="E82" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F82" s="6" t="s">
+      <c r="E82" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F82" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="G82" s="7">
+      <c r="G82" s="11">
         <v>42802</v>
       </c>
-      <c r="H82" s="6"/>
+      <c r="H82" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C83" s="10">
         <v>923381</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="10">
         <v>931795</v>
       </c>
-      <c r="E83" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F83" s="6" t="s">
+      <c r="E83" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F83" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="G83" s="7">
+      <c r="G83" s="11">
         <v>42850</v>
       </c>
-      <c r="H83" s="6"/>
+      <c r="H83" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
-      <c r="B84" s="6" t="s">
+      <c r="B84" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="10">
         <v>935738</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="10">
         <v>939392</v>
       </c>
-      <c r="E84" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F84" s="6" t="s">
+      <c r="E84" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F84" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="G84" s="7">
+      <c r="G84" s="11">
         <v>42803</v>
       </c>
-      <c r="H84" s="6"/>
+      <c r="H84" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C85" s="10">
         <v>908403</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85" s="10">
         <v>936528</v>
       </c>
-      <c r="E85" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F85" s="6" t="s">
+      <c r="E85" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F85" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="G85" s="7">
+      <c r="G85" s="11">
         <v>42804</v>
       </c>
-      <c r="H85" s="6"/>
+      <c r="H85" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="8">
         <v>935078</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86" s="8">
         <v>907244</v>
       </c>
-      <c r="E86" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F86" s="6" t="s">
+      <c r="E86" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F86" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G86" s="7">
+      <c r="G86" s="12">
         <v>42808</v>
       </c>
-      <c r="H86" s="6"/>
+      <c r="H86" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="6">
+      <c r="C87" s="8">
         <v>923234</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D87" s="8">
         <v>923893</v>
       </c>
-      <c r="E87" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F87" s="6" t="s">
+      <c r="E87" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F87" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G87" s="8">
         <v>3172017</v>
       </c>
-      <c r="H87" s="6"/>
+      <c r="H87" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C88" s="6">
+      <c r="C88" s="8">
         <v>923234</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D88" s="8">
         <v>924191</v>
       </c>
-      <c r="E88" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F88" s="6" t="s">
+      <c r="E88" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F88" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="G88" s="6">
+      <c r="G88" s="8">
         <v>3302017</v>
       </c>
-      <c r="H88" s="6"/>
+      <c r="H88" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="6">
+      <c r="C89" s="10">
         <v>935738</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D89" s="10">
         <v>939392</v>
       </c>
-      <c r="E89" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F89" s="6" t="s">
+      <c r="E89" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F89" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G89" s="6">
+      <c r="G89" s="10">
         <v>3202017</v>
       </c>
-      <c r="H89" s="6"/>
+      <c r="H89" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C90" s="6">
+      <c r="C90" s="10">
         <v>910322</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90" s="10">
         <v>936519</v>
       </c>
-      <c r="E90" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F90" s="6" t="s">
+      <c r="E90" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F90" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90" s="10">
         <v>3202017</v>
       </c>
-      <c r="H90" s="6"/>
+      <c r="H90" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C91" s="6">
+      <c r="C91" s="8">
         <v>905617</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D91" s="8">
         <v>905917</v>
       </c>
-      <c r="E91" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F91" s="6" t="s">
+      <c r="E91" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F91" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="G91" s="6">
+      <c r="G91" s="8">
         <v>3202017</v>
       </c>
-      <c r="H91" s="6"/>
+      <c r="H91" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C92" s="6">
+      <c r="C92" s="8">
         <v>935040</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92" s="8">
         <v>930695</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F92" s="6" t="s">
+      <c r="E92" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F92" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="G92" s="6">
+      <c r="G92" s="8">
         <v>3262017</v>
       </c>
-      <c r="H92" s="6"/>
+      <c r="H92" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C93" s="6">
+      <c r="C93" s="10">
         <v>936386</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D93" s="10">
         <v>918938</v>
       </c>
-      <c r="E93" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F93" s="6" t="s">
+      <c r="E93" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F93" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="G93" s="6">
+      <c r="G93" s="10">
         <v>3242017</v>
       </c>
-      <c r="H93" s="6"/>
+      <c r="H93" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
-      <c r="B94" s="6" t="s">
+      <c r="B94" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C94" s="6">
+      <c r="C94" s="8">
         <v>936105</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94" s="8">
         <v>943297</v>
       </c>
-      <c r="E94" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F94" s="6" t="s">
+      <c r="E94" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F94" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G94" s="6">
+      <c r="G94" s="8">
         <v>3252017</v>
       </c>
-      <c r="H94" s="6"/>
+      <c r="H94" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C95" s="6">
+      <c r="C95" s="10">
         <v>912885</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D95" s="10">
         <v>936547</v>
       </c>
-      <c r="E95" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F95" s="6" t="s">
+      <c r="E95" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F95" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="G95" s="6">
+      <c r="G95" s="10">
         <v>3252017</v>
       </c>
-      <c r="H95" s="6"/>
+      <c r="H95" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C96" s="6">
+      <c r="C96" s="8">
         <v>904122</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96" s="8">
         <v>905920</v>
       </c>
-      <c r="E96" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F96" s="6" t="s">
+      <c r="E96" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F96" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="G96" s="6">
+      <c r="G96" s="8">
         <v>3242017</v>
       </c>
-      <c r="H96" s="6"/>
+      <c r="H96" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C97" s="6">
+      <c r="C97" s="10">
         <v>900509</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="10">
         <v>943328</v>
       </c>
-      <c r="E97" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F97" s="6" t="s">
+      <c r="E97" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F97" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="G97" s="6">
+      <c r="G97" s="10">
         <v>3272017</v>
       </c>
-      <c r="H97" s="6"/>
+      <c r="H97" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="6">
+      <c r="C98" s="8">
         <v>900504</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="8">
         <v>913334</v>
       </c>
-      <c r="E98" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F98" s="6" t="s">
+      <c r="E98" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F98" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="G98" s="6">
+      <c r="G98" s="8">
         <v>3172017</v>
       </c>
-      <c r="H98" s="6"/>
+      <c r="H98" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C99" s="6">
+      <c r="C99" s="8">
         <v>925605</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D99" s="8">
         <v>943319</v>
       </c>
-      <c r="E99" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F99" s="6" t="s">
+      <c r="E99" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="G99" s="6">
+      <c r="G99" s="8">
         <v>3282017</v>
       </c>
-      <c r="H99" s="6"/>
+      <c r="H99" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
-      <c r="B100" s="6" t="s">
+      <c r="B100" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C100" s="6">
+      <c r="C100" s="8">
         <v>936993</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100" s="8">
         <v>916665</v>
       </c>
-      <c r="E100" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F100" s="6" t="s">
+      <c r="E100" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F100" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="G100" s="6">
+      <c r="G100" s="8">
         <v>3292017</v>
       </c>
-      <c r="H100" s="6"/>
+      <c r="H100" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C101" s="6">
+      <c r="C101" s="10">
         <v>935024</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="10">
         <v>904333</v>
       </c>
-      <c r="E101" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F101" s="6" t="s">
+      <c r="E101" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F101" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="G101" s="6">
+      <c r="G101" s="10">
         <v>3292017</v>
       </c>
-      <c r="H101" s="6"/>
+      <c r="H101" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
-      <c r="B102" s="6" t="s">
+      <c r="B102" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C102" s="6">
+      <c r="C102" s="8">
         <v>900504</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D102" s="8">
         <v>913334</v>
       </c>
-      <c r="E102" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F102" s="6" t="s">
+      <c r="E102" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F102" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="G102" s="6">
+      <c r="G102" s="8">
         <v>3292017</v>
       </c>
-      <c r="H102" s="6"/>
+      <c r="H102" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C103" s="6">
+      <c r="C103" s="8">
         <v>923234</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D103" s="8">
         <v>923893</v>
       </c>
-      <c r="E103" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F103" s="6" t="s">
+      <c r="E103" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F103" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G103" s="6">
+      <c r="G103" s="8">
         <v>3302017</v>
       </c>
-      <c r="H103" s="6"/>
+      <c r="H103" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C104" s="6">
+      <c r="C104" s="8">
         <v>935342</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D104" s="8">
         <v>915833</v>
       </c>
-      <c r="E104" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F104" s="6" t="s">
+      <c r="E104" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F104" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="G104" s="6">
+      <c r="G104" s="8">
         <v>4012017</v>
       </c>
-      <c r="H104" s="6"/>
+      <c r="H104" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C105" s="6">
+      <c r="C105" s="10">
         <v>929488</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D105" s="10">
         <v>946645</v>
       </c>
-      <c r="E105" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F105" s="6" t="s">
+      <c r="E105" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F105" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G105" s="6">
+      <c r="G105" s="10">
         <v>3302017</v>
       </c>
-      <c r="H105" s="6"/>
+      <c r="H105" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C106" s="6">
+      <c r="C106" s="10">
         <v>947660</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D106" s="10">
         <v>930697</v>
       </c>
-      <c r="E106" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F106" s="6" t="s">
+      <c r="E106" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F106" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="G106" s="6">
+      <c r="G106" s="10">
         <v>3302017</v>
       </c>
-      <c r="H106" s="6"/>
+      <c r="H106" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C107" s="6">
+      <c r="C107" s="10">
         <v>923234</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D107" s="10">
         <v>923893</v>
       </c>
-      <c r="E107" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F107" s="6" t="s">
+      <c r="E107" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F107" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="G107" s="6">
+      <c r="G107" s="10">
         <v>4012017</v>
       </c>
-      <c r="H107" s="6"/>
+      <c r="H107" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C108" s="6">
+      <c r="C108" s="10">
         <v>900819</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D108" s="10">
         <v>936526</v>
       </c>
-      <c r="E108" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F108" s="6" t="s">
+      <c r="E108" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F108" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="G108" s="6">
+      <c r="G108" s="10">
         <v>3312017</v>
       </c>
-      <c r="H108" s="6"/>
+      <c r="H108" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C109" s="6">
+      <c r="C109" s="8">
         <v>910322</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D109" s="8">
         <v>936519</v>
       </c>
-      <c r="E109" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F109" s="6" t="s">
+      <c r="E109" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F109" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G109" s="6">
+      <c r="G109" s="8">
         <v>4012017</v>
       </c>
-      <c r="H109" s="6"/>
+      <c r="H109" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
-      <c r="B110" s="6" t="s">
+      <c r="B110" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="6">
+      <c r="C110" s="10">
         <v>935342</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D110" s="10">
         <v>915833</v>
       </c>
-      <c r="E110" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F110" s="6" t="s">
+      <c r="E110" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F110" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G110" s="6">
+      <c r="G110" s="10">
         <v>4032017</v>
       </c>
-      <c r="H110" s="6"/>
+      <c r="H110" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
-      <c r="B111" s="6" t="s">
+      <c r="B111" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="C111" s="6">
+      <c r="C111" s="10">
         <v>900504</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D111" s="10">
         <v>913334</v>
       </c>
-      <c r="E111" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F111" s="6" t="s">
+      <c r="E111" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F111" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="G111" s="6">
+      <c r="G111" s="10">
         <v>4032017</v>
       </c>
-      <c r="H111" s="6"/>
+      <c r="H111" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
-      <c r="B112" s="6" t="s">
+      <c r="B112" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="C112" s="6">
+      <c r="C112" s="8">
         <v>936119</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D112" s="8">
         <v>936546</v>
       </c>
-      <c r="E112" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F112" s="6" t="s">
+      <c r="E112" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F112" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="G112" s="6">
+      <c r="G112" s="8">
         <v>4032017</v>
       </c>
-      <c r="H112" s="6"/>
+      <c r="H112" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
-      <c r="B113" s="6" t="s">
+      <c r="B113" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C113" s="6">
+      <c r="C113" s="10">
         <v>904176</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D113" s="10">
         <v>926379</v>
       </c>
-      <c r="E113" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F113" s="6" t="s">
+      <c r="E113" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F113" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="G113" s="6">
+      <c r="G113" s="10">
         <v>4042017</v>
       </c>
-      <c r="H113" s="6"/>
+      <c r="H113" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
-      <c r="B114" s="6" t="s">
+      <c r="B114" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C114" s="6">
+      <c r="C114" s="10">
         <v>936119</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D114" s="10">
         <v>936546</v>
       </c>
-      <c r="E114" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F114" s="6" t="s">
+      <c r="E114" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F114" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G114" s="6">
+      <c r="G114" s="10">
         <v>4042017</v>
       </c>
-      <c r="H114" s="6"/>
+      <c r="H114" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
-      <c r="B115" s="6" t="s">
+      <c r="B115" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C115" s="6">
+      <c r="C115" s="10">
         <v>908403</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D115" s="10">
         <v>936521</v>
       </c>
-      <c r="E115" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F115" s="6" t="s">
+      <c r="E115" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F115" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="G115" s="6">
+      <c r="G115" s="10">
         <v>4032017</v>
       </c>
-      <c r="H115" s="6"/>
+      <c r="H115" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
-      <c r="B116" s="6" t="s">
+      <c r="B116" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C116" s="6">
+      <c r="C116" s="8">
         <v>915497</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D116" s="8">
         <v>946645</v>
       </c>
-      <c r="E116" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F116" s="6" t="s">
+      <c r="E116" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F116" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="G116" s="6">
+      <c r="G116" s="8">
         <v>4042017</v>
       </c>
-      <c r="H116" s="6"/>
+      <c r="H116" s="7" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
-      <c r="B117" s="6" t="s">
+      <c r="B117" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="C117" s="6">
+      <c r="C117" s="10">
         <v>936119</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D117" s="10">
         <v>936540</v>
       </c>
-      <c r="E117" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F117" s="6" t="s">
+      <c r="E117" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F117" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="G117" s="6">
+      <c r="G117" s="10">
         <v>4042017</v>
       </c>
-      <c r="H117" s="6"/>
+      <c r="H117" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
-      <c r="B118" s="6" t="s">
+      <c r="B118" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="C118" s="6">
+      <c r="C118" s="10">
         <v>908403</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D118" s="10">
         <v>906345</v>
       </c>
-      <c r="E118" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F118" s="6" t="s">
+      <c r="E118" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F118" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="G118" s="6">
+      <c r="G118" s="10">
         <v>4062017</v>
       </c>
-      <c r="H118" s="6"/>
+      <c r="H118" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
-      <c r="B119" s="6" t="s">
+      <c r="B119" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="C119" s="6">
+      <c r="C119" s="10">
         <v>900504</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D119" s="10">
         <v>902108</v>
       </c>
-      <c r="E119" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F119" s="6" t="s">
+      <c r="E119" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F119" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="G119" s="6">
+      <c r="G119" s="10">
         <v>4062017</v>
       </c>
-      <c r="H119" s="6"/>
+      <c r="H119" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
-      <c r="B120" s="6" t="s">
+      <c r="B120" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C120" s="6">
+      <c r="C120" s="10">
         <v>900504</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D120" s="10">
         <v>902108</v>
       </c>
-      <c r="E120" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F120" s="6" t="s">
+      <c r="E120" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F120" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="G120" s="6">
+      <c r="G120" s="10">
         <v>4082017</v>
       </c>
-      <c r="H120" s="6"/>
+      <c r="H120" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
-      <c r="B121" s="6" t="s">
+      <c r="B121" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C121" s="6">
+      <c r="C121" s="8">
         <v>937376</v>
       </c>
-      <c r="D121" s="6">
+      <c r="D121" s="8">
         <v>943301</v>
       </c>
-      <c r="E121" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F121" s="6" t="s">
+      <c r="E121" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F121" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="G121" s="6">
+      <c r="G121" s="8">
         <v>4082017</v>
       </c>
-      <c r="H121" s="6"/>
+      <c r="H121" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
-      <c r="B122" s="6" t="s">
+      <c r="B122" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C122" s="6">
+      <c r="C122" s="10">
         <v>915497</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D122" s="10">
         <v>946645</v>
       </c>
-      <c r="E122" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F122" s="6" t="s">
+      <c r="E122" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F122" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="G122" s="6">
+      <c r="G122" s="10">
         <v>4062017</v>
       </c>
-      <c r="H122" s="6"/>
+      <c r="H122" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C123" s="6">
+      <c r="C123" s="8">
         <v>936768</v>
       </c>
-      <c r="D123" s="6">
+      <c r="D123" s="8">
         <v>939367</v>
       </c>
-      <c r="E123" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F123" s="6" t="s">
+      <c r="E123" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F123" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="G123" s="6">
+      <c r="G123" s="8">
         <v>4072017</v>
       </c>
-      <c r="H123" s="6"/>
+      <c r="H123" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C124" s="6">
+      <c r="C124" s="10">
         <v>937109</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D124" s="10">
         <v>943297</v>
       </c>
-      <c r="E124" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F124" s="6" t="s">
+      <c r="E124" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F124" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="G124" s="6">
+      <c r="G124" s="10">
         <v>4072017</v>
       </c>
-      <c r="H124" s="6"/>
+      <c r="H124" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
-      <c r="B125" s="6" t="s">
+      <c r="B125" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="C125" s="6">
+      <c r="C125" s="8">
         <v>932329</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D125" s="8">
         <v>907307</v>
       </c>
-      <c r="E125" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F125" s="6" t="s">
+      <c r="E125" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F125" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="G125" s="6">
+      <c r="G125" s="8">
         <v>4102017</v>
       </c>
-      <c r="H125" s="6"/>
+      <c r="H125" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
-      <c r="B126" s="6" t="s">
+      <c r="B126" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="C126" s="6">
+      <c r="C126" s="8">
         <v>900504</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D126" s="8">
         <v>913334</v>
       </c>
-      <c r="E126" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F126" s="6" t="s">
+      <c r="E126" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F126" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="G126" s="6">
+      <c r="G126" s="8">
         <v>4092017</v>
       </c>
-      <c r="H126" s="6"/>
+      <c r="H126" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
-      <c r="B127" s="6" t="s">
+      <c r="B127" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C127" s="6">
+      <c r="C127" s="10">
         <v>931142</v>
       </c>
-      <c r="D127" s="6">
+      <c r="D127" s="10">
         <v>920759</v>
       </c>
-      <c r="E127" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F127" s="6" t="s">
+      <c r="E127" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F127" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G127" s="6">
+      <c r="G127" s="10">
         <v>4092017</v>
       </c>
-      <c r="H127" s="6"/>
+      <c r="H127" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="6"/>
-      <c r="B128" s="6" t="s">
+      <c r="B128" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="C128" s="6">
+      <c r="C128" s="10">
         <v>915497</v>
       </c>
-      <c r="D128" s="6">
+      <c r="D128" s="10">
         <v>946645</v>
       </c>
-      <c r="E128" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F128" s="6" t="s">
+      <c r="E128" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F128" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="G128" s="6">
+      <c r="G128" s="10">
         <v>4082017</v>
       </c>
-      <c r="H128" s="6"/>
+      <c r="H128" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
-      <c r="B129" s="6" t="s">
+      <c r="B129" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="C129" s="6">
+      <c r="C129" s="10">
         <v>947660</v>
       </c>
-      <c r="D129" s="6">
+      <c r="D129" s="10">
         <v>930697</v>
       </c>
-      <c r="E129" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F129" s="6" t="s">
+      <c r="E129" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F129" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="G129" s="6">
+      <c r="G129" s="10">
         <v>3302017</v>
       </c>
-      <c r="H129" s="6"/>
+      <c r="H129" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="6"/>
-      <c r="B130" s="6" t="s">
+      <c r="B130" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="C130" s="6">
+      <c r="C130" s="8">
         <v>932329</v>
       </c>
-      <c r="D130" s="6">
+      <c r="D130" s="8">
         <v>907307</v>
       </c>
-      <c r="E130" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F130" s="6" t="s">
+      <c r="E130" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F130" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G130" s="6">
+      <c r="G130" s="8">
         <v>4102017</v>
       </c>
-      <c r="H130" s="6"/>
+      <c r="H130" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="6"/>
-      <c r="B131" s="6" t="s">
+      <c r="B131" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C131" s="6">
+      <c r="C131" s="10">
         <v>936119</v>
       </c>
-      <c r="D131" s="6">
+      <c r="D131" s="10">
         <v>936546</v>
       </c>
-      <c r="E131" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F131" s="6" t="s">
+      <c r="E131" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F131" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="G131" s="6">
+      <c r="G131" s="10">
         <v>4102017</v>
       </c>
-      <c r="H131" s="6"/>
+      <c r="H131" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="6"/>
-      <c r="B132" s="6" t="s">
+      <c r="B132" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C132" s="6">
+      <c r="C132" s="10">
         <v>936119</v>
       </c>
-      <c r="D132" s="6">
+      <c r="D132" s="10">
         <v>936546</v>
       </c>
-      <c r="E132" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F132" s="6" t="s">
+      <c r="E132" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F132" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="G132" s="6">
+      <c r="G132" s="10">
         <v>4102017</v>
       </c>
-      <c r="H132" s="6"/>
+      <c r="H132" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
-      <c r="B133" s="6" t="s">
+      <c r="B133" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="C133" s="6">
+      <c r="C133" s="10">
         <v>937109</v>
       </c>
-      <c r="D133" s="6">
+      <c r="D133" s="10">
         <v>908539</v>
       </c>
-      <c r="E133" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F133" s="6" t="s">
+      <c r="E133" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F133" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="G133" s="6">
+      <c r="G133" s="10">
         <v>4102017</v>
       </c>
-      <c r="H133" s="6"/>
+      <c r="H133" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="6"/>
-      <c r="B134" s="6" t="s">
+      <c r="B134" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="C134" s="6">
+      <c r="C134" s="10">
         <v>921993</v>
       </c>
-      <c r="D134" s="6">
+      <c r="D134" s="10">
         <v>920761</v>
       </c>
-      <c r="E134" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F134" s="6" t="s">
+      <c r="E134" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F134" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="G134" s="6">
+      <c r="G134" s="10">
         <v>3312017</v>
       </c>
-      <c r="H134" s="6"/>
+      <c r="H134" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="6"/>
-      <c r="B135" s="6" t="s">
+      <c r="B135" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="C135" s="6">
+      <c r="C135" s="10">
         <v>925605</v>
       </c>
-      <c r="D135" s="6">
+      <c r="D135" s="10">
         <v>943319</v>
       </c>
-      <c r="E135" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F135" s="6" t="s">
+      <c r="E135" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F135" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G135" s="6">
+      <c r="G135" s="10">
         <v>4112017</v>
       </c>
-      <c r="H135" s="6"/>
+      <c r="H135" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="6"/>
-      <c r="B136" s="6" t="s">
+      <c r="B136" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="C136" s="6">
+      <c r="C136" s="10">
         <v>921419</v>
       </c>
-      <c r="D136" s="6">
+      <c r="D136" s="10">
         <v>945092</v>
       </c>
-      <c r="E136" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F136" s="6" t="s">
+      <c r="E136" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F136" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="G136" s="6">
+      <c r="G136" s="10">
         <v>4122017</v>
       </c>
-      <c r="H136" s="6"/>
+      <c r="H136" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
-      <c r="B137" s="6" t="s">
+      <c r="B137" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="C137" s="6">
+      <c r="C137" s="10">
         <v>936119</v>
       </c>
-      <c r="D137" s="6">
+      <c r="D137" s="10">
         <v>936546</v>
       </c>
-      <c r="E137" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F137" s="6" t="s">
+      <c r="E137" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F137" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="G137" s="6">
+      <c r="G137" s="10">
         <v>4112017</v>
       </c>
-      <c r="H137" s="6"/>
+      <c r="H137" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
-      <c r="B138" s="6" t="s">
+      <c r="B138" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="C138" s="6">
+      <c r="C138" s="10">
         <v>936119</v>
       </c>
-      <c r="D138" s="6">
+      <c r="D138" s="10">
         <v>936546</v>
       </c>
-      <c r="E138" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F138" s="6" t="s">
+      <c r="E138" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F138" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G138" s="6">
+      <c r="G138" s="10">
         <v>4122017</v>
       </c>
-      <c r="H138" s="6"/>
+      <c r="H138" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
-      <c r="B139" s="6" t="s">
+      <c r="B139" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="C139" s="6">
+      <c r="C139" s="10">
         <v>936768</v>
       </c>
-      <c r="D139" s="6">
+      <c r="D139" s="10">
         <v>939367</v>
       </c>
-      <c r="E139" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F139" s="6" t="s">
+      <c r="E139" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F139" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="G139" s="6">
+      <c r="G139" s="10">
         <v>2222017</v>
       </c>
-      <c r="H139" s="6"/>
+      <c r="H139" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="6"/>
-      <c r="B140" s="6" t="s">
+      <c r="B140" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="C140" s="6">
+      <c r="C140" s="8">
         <v>919753</v>
       </c>
-      <c r="D140" s="6">
+      <c r="D140" s="8">
         <v>936489</v>
       </c>
-      <c r="E140" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F140" s="6" t="s">
+      <c r="E140" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F140" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="G140" s="6">
+      <c r="G140" s="8">
         <v>4132017</v>
       </c>
-      <c r="H140" s="6"/>
+      <c r="H140" s="7" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
-      <c r="B141" s="6" t="s">
+      <c r="B141" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="C141" s="6">
+      <c r="C141" s="8">
         <v>913868</v>
       </c>
-      <c r="D141" s="6">
+      <c r="D141" s="8">
         <v>936528</v>
       </c>
-      <c r="E141" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F141" s="6" t="s">
+      <c r="E141" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F141" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="G141" s="6">
+      <c r="G141" s="8">
         <v>4142017</v>
       </c>
-      <c r="H141" s="6"/>
+      <c r="H141" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
-      <c r="B142" s="6" t="s">
+      <c r="B142" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="C142" s="6">
+      <c r="C142" s="10">
         <v>913181</v>
       </c>
-      <c r="D142" s="6">
+      <c r="D142" s="10">
         <v>933752</v>
       </c>
-      <c r="E142" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F142" s="6" t="s">
+      <c r="E142" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F142" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="G142" s="6">
+      <c r="G142" s="10">
         <v>4132017</v>
       </c>
-      <c r="H142" s="6"/>
+      <c r="H142" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
-      <c r="B143" s="6" t="s">
+      <c r="B143" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="C143" s="6">
+      <c r="C143" s="8">
         <v>908403</v>
       </c>
-      <c r="D143" s="6">
+      <c r="D143" s="8">
         <v>936521</v>
       </c>
-      <c r="E143" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F143" s="6" t="s">
+      <c r="E143" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F143" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="G143" s="6">
+      <c r="G143" s="8">
         <v>4122017</v>
       </c>
-      <c r="H143" s="6"/>
+      <c r="H143" s="7" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
-      <c r="B144" s="6" t="s">
+      <c r="B144" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C144" s="6">
+      <c r="C144" s="10">
         <v>913181</v>
       </c>
-      <c r="D144" s="6">
+      <c r="D144" s="10">
         <v>939939</v>
       </c>
-      <c r="E144" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F144" s="6" t="s">
+      <c r="E144" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F144" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G144" s="6">
+      <c r="G144" s="10">
         <v>4132017</v>
       </c>
-      <c r="H144" s="6"/>
+      <c r="H144" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
-      <c r="B145" s="6" t="s">
+      <c r="B145" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C145" s="6">
+      <c r="C145" s="10">
         <v>900504</v>
       </c>
-      <c r="D145" s="6">
+      <c r="D145" s="10">
         <v>902108</v>
       </c>
-      <c r="E145" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F145" s="6" t="s">
+      <c r="E145" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F145" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="G145" s="6">
+      <c r="G145" s="10">
         <v>4142017</v>
       </c>
-      <c r="H145" s="6"/>
+      <c r="H145" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>
-      <c r="B146" s="6" t="s">
+      <c r="B146" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C146" s="6">
+      <c r="C146" s="8">
         <v>904122</v>
       </c>
-      <c r="D146" s="6">
+      <c r="D146" s="8">
         <v>905912</v>
       </c>
-      <c r="E146" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F146" s="6" t="s">
+      <c r="E146" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F146" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G146" s="6">
+      <c r="G146" s="8">
         <v>4142017</v>
       </c>
-      <c r="H146" s="6"/>
+      <c r="H146" s="7" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
-      <c r="B147" s="6" t="s">
+      <c r="B147" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C147" s="6">
+      <c r="C147" s="10">
         <v>937109</v>
       </c>
-      <c r="D147" s="6">
+      <c r="D147" s="10">
         <v>936533</v>
       </c>
-      <c r="E147" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F147" s="6" t="s">
+      <c r="E147" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F147" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="G147" s="6">
+      <c r="G147" s="10">
         <v>4142017</v>
       </c>
-      <c r="H147" s="6"/>
+      <c r="H147" s="9" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
@@ -8554,140 +8708,140 @@
       </c>
     </row>
     <row r="265" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B265" s="14" t="s">
+      <c r="B265" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="C265" s="15">
+      <c r="C265" s="14">
         <v>943674</v>
       </c>
-      <c r="D265" s="15">
+      <c r="D265" s="14">
         <v>923693</v>
       </c>
-      <c r="E265" s="15" t="s">
+      <c r="E265" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F265" s="15" t="s">
+      <c r="F265" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="G265" s="15">
+      <c r="G265" s="14">
         <v>4192017</v>
       </c>
-      <c r="H265" s="14" t="s">
+      <c r="H265" s="13" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="266" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B266" s="16" t="s">
+      <c r="B266" s="15" t="s">
         <v>485</v>
       </c>
-      <c r="C266" s="17">
+      <c r="C266" s="16">
         <v>949538</v>
       </c>
-      <c r="D266" s="17">
+      <c r="D266" s="16">
         <v>949538</v>
       </c>
-      <c r="E266" s="17" t="s">
+      <c r="E266" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F266" s="17" t="s">
+      <c r="F266" s="16" t="s">
         <v>486</v>
       </c>
-      <c r="G266" s="17">
+      <c r="G266" s="16">
         <v>4262017</v>
       </c>
-      <c r="H266" s="16" t="s">
+      <c r="H266" s="15" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="267" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B267" s="16" t="s">
+      <c r="B267" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="C267" s="17">
+      <c r="C267" s="16">
         <v>935727</v>
       </c>
-      <c r="D267" s="17">
+      <c r="D267" s="16">
         <v>920176</v>
       </c>
-      <c r="E267" s="17" t="s">
+      <c r="E267" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F267" s="17" t="s">
+      <c r="F267" s="16" t="s">
         <v>488</v>
       </c>
-      <c r="G267" s="17">
+      <c r="G267" s="16">
         <v>5102017</v>
       </c>
-      <c r="H267" s="16" t="s">
+      <c r="H267" s="15" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="268" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B268" s="16" t="s">
+      <c r="B268" s="15" t="s">
         <v>489</v>
       </c>
-      <c r="C268" s="17">
+      <c r="C268" s="16">
         <v>922113</v>
       </c>
-      <c r="D268" s="17">
+      <c r="D268" s="16">
         <v>936469</v>
       </c>
-      <c r="E268" s="17" t="s">
+      <c r="E268" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F268" s="17" t="s">
+      <c r="F268" s="16" t="s">
         <v>490</v>
       </c>
-      <c r="G268" s="17">
+      <c r="G268" s="16">
         <v>4272017</v>
       </c>
-      <c r="H268" s="16" t="s">
+      <c r="H268" s="15" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="269" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B269" s="14" t="s">
+      <c r="B269" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="C269" s="15">
+      <c r="C269" s="14">
         <v>944565</v>
       </c>
-      <c r="D269" s="15">
+      <c r="D269" s="14">
         <v>936475</v>
       </c>
-      <c r="E269" s="15" t="s">
+      <c r="E269" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F269" s="15" t="s">
+      <c r="F269" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="G269" s="15">
+      <c r="G269" s="14">
         <v>4292017</v>
       </c>
-      <c r="H269" s="14" t="s">
+      <c r="H269" s="13" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="270" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B270" s="14" t="s">
+      <c r="B270" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C270" s="15">
+      <c r="C270" s="14">
         <v>917687</v>
       </c>
-      <c r="D270" s="15">
+      <c r="D270" s="14">
         <v>920157</v>
       </c>
-      <c r="E270" s="15" t="s">
+      <c r="E270" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F270" s="15" t="s">
+      <c r="F270" s="14" t="s">
         <v>493</v>
       </c>
-      <c r="G270" s="15">
+      <c r="G270" s="14">
         <v>5042017</v>
       </c>
-      <c r="H270" s="14" t="s">
+      <c r="H270" s="13" t="s">
         <v>752</v>
       </c>
     </row>

</xml_diff>